<commit_message>
docs: Update state machine transitions spreadsheet
</commit_message>
<xml_diff>
--- a/Guide/HEAR Software/Flight Modes/state_machine_transitions.xlsx
+++ b/Guide/HEAR Software/Flight Modes/state_machine_transitions.xlsx
@@ -14,7 +14,7 @@
     <sheet name="other_todo" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">state_machine_transitions!$B$29:$N$172</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">state_machine_transitions!$B$29:$O$172</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="237">
   <si>
     <t xml:space="preserve">Mission Manager State</t>
   </si>
@@ -353,6 +353,9 @@
   </si>
   <si>
     <t xml:space="preserve">[PAUSED,CANCELED,LOADED]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Follow queueing configs. Once mission at tip is [cancelled, completed or failed], deque and load the next mission</t>
   </si>
   <si>
     <t xml:space="preserve">“”</t>
@@ -1232,12 +1235,12 @@
       <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="29.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="29.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.67"/>
   </cols>
@@ -1656,13 +1659,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N172"/>
+  <dimension ref="A1:O172"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E48" activeCellId="0" sqref="E48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="27.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="32.3"/>
@@ -1671,12 +1674,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="27" width="6.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="27" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="27" width="9.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="27" width="9.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="27" width="17.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="27" width="28.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="27" width="21.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="27" width="43.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="27" width="15.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="27" width="9.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="27" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="27" width="28.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="27" width="21.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="27" width="43.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="27" width="15.49"/>
   </cols>
   <sheetData>
     <row r="1" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1695,6 +1698,7 @@
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
       <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
     </row>
     <row r="2" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="29"/>
@@ -1712,6 +1716,7 @@
       <c r="L2" s="30"/>
       <c r="M2" s="30"/>
       <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
     </row>
     <row r="3" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="29"/>
@@ -1729,6 +1734,7 @@
       <c r="L3" s="30"/>
       <c r="M3" s="30"/>
       <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
     </row>
     <row r="4" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="29"/>
@@ -1746,6 +1752,7 @@
       <c r="L4" s="30"/>
       <c r="M4" s="30"/>
       <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
     </row>
     <row r="5" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="29"/>
@@ -1763,6 +1770,7 @@
       <c r="L5" s="30"/>
       <c r="M5" s="30"/>
       <c r="N5" s="30"/>
+      <c r="O5" s="30"/>
     </row>
     <row r="6" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="29"/>
@@ -1780,6 +1788,7 @@
       <c r="L6" s="30"/>
       <c r="M6" s="30"/>
       <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
     </row>
     <row r="7" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="29"/>
@@ -1795,6 +1804,7 @@
       <c r="L7" s="30"/>
       <c r="M7" s="30"/>
       <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
     </row>
     <row r="8" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="29" t="s">
@@ -1812,6 +1822,7 @@
       <c r="L8" s="30"/>
       <c r="M8" s="30"/>
       <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
     </row>
     <row r="9" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="29"/>
@@ -1829,6 +1840,7 @@
       <c r="L9" s="30"/>
       <c r="M9" s="30"/>
       <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
     </row>
     <row r="10" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="29"/>
@@ -1846,6 +1858,7 @@
       <c r="L10" s="30"/>
       <c r="M10" s="30"/>
       <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
     </row>
     <row r="11" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="29"/>
@@ -1861,6 +1874,7 @@
       <c r="L11" s="30"/>
       <c r="M11" s="30"/>
       <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
     </row>
     <row r="12" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="29"/>
@@ -1878,6 +1892,7 @@
       <c r="L12" s="30"/>
       <c r="M12" s="30"/>
       <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
     </row>
     <row r="13" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="29"/>
@@ -1895,6 +1910,7 @@
       <c r="L13" s="30"/>
       <c r="M13" s="30"/>
       <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
     </row>
     <row r="14" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="29" t="s">
@@ -1912,6 +1928,7 @@
       <c r="L14" s="30"/>
       <c r="M14" s="30"/>
       <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
     </row>
     <row r="15" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="29"/>
@@ -1929,6 +1946,7 @@
       <c r="L15" s="30"/>
       <c r="M15" s="30"/>
       <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
     </row>
     <row r="16" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="29"/>
@@ -1944,6 +1962,7 @@
       <c r="L16" s="30"/>
       <c r="M16" s="30"/>
       <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
     </row>
     <row r="17" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="29"/>
@@ -1959,6 +1978,7 @@
       <c r="L17" s="30"/>
       <c r="M17" s="30"/>
       <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
     </row>
     <row r="18" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="31" t="s">
@@ -1982,6 +2002,7 @@
       <c r="L18" s="30"/>
       <c r="M18" s="30"/>
       <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
     </row>
     <row r="19" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="31" t="s">
@@ -2005,6 +2026,7 @@
       <c r="L19" s="30"/>
       <c r="M19" s="30"/>
       <c r="N19" s="30"/>
+      <c r="O19" s="30"/>
     </row>
     <row r="20" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="32" t="s">
@@ -2028,6 +2050,7 @@
       <c r="L20" s="30"/>
       <c r="M20" s="30"/>
       <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
     </row>
     <row r="21" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="32"/>
@@ -2047,6 +2070,7 @@
       <c r="L21" s="30"/>
       <c r="M21" s="30"/>
       <c r="N21" s="30"/>
+      <c r="O21" s="30"/>
     </row>
     <row r="22" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="31"/>
@@ -2066,6 +2090,7 @@
       <c r="L22" s="30"/>
       <c r="M22" s="30"/>
       <c r="N22" s="30"/>
+      <c r="O22" s="30"/>
     </row>
     <row r="23" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="31"/>
@@ -2083,6 +2108,7 @@
       <c r="L23" s="30"/>
       <c r="M23" s="30"/>
       <c r="N23" s="30"/>
+      <c r="O23" s="30"/>
     </row>
     <row r="24" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="31"/>
@@ -2100,6 +2126,7 @@
       <c r="L24" s="30"/>
       <c r="M24" s="30"/>
       <c r="N24" s="30"/>
+      <c r="O24" s="30"/>
     </row>
     <row r="25" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="31"/>
@@ -2117,6 +2144,7 @@
       <c r="L25" s="30"/>
       <c r="M25" s="30"/>
       <c r="N25" s="30"/>
+      <c r="O25" s="30"/>
     </row>
     <row r="26" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="31"/>
@@ -2134,6 +2162,7 @@
       <c r="L26" s="30"/>
       <c r="M26" s="30"/>
       <c r="N26" s="30"/>
+      <c r="O26" s="30"/>
     </row>
     <row r="27" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="31"/>
@@ -2151,6 +2180,7 @@
       <c r="L27" s="30"/>
       <c r="M27" s="30"/>
       <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="4"/>
@@ -2166,6 +2196,7 @@
       <c r="L28" s="33"/>
       <c r="M28" s="33"/>
       <c r="N28" s="33"/>
+      <c r="O28" s="33"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
@@ -2196,18 +2227,21 @@
         <v>94</v>
       </c>
       <c r="J29" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="K29" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="K29" s="33" t="s">
+      <c r="L29" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="L29" s="33" t="s">
+      <c r="M29" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="M29" s="33" t="s">
+      <c r="N29" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="N29" s="33" t="s">
+      <c r="O29" s="33" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2219,7 +2253,7 @@
       <c r="C30" s="34"/>
       <c r="D30" s="34"/>
       <c r="E30" s="34"/>
-      <c r="M30" s="35"/>
+      <c r="N30" s="35"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="36" t="n">
@@ -2246,18 +2280,21 @@
       <c r="I31" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="J31" s="37" t="s">
+      <c r="J31" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K31" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="K31" s="37" t="s">
+      <c r="L31" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="L31" s="39" t="s">
+      <c r="M31" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="M31" s="35"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N31" s="35"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="36" t="n">
         <v>3</v>
       </c>
@@ -2282,14 +2319,17 @@
       <c r="I32" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="J32" s="0"/>
+      <c r="J32" s="27" t="s">
+        <v>85</v>
+      </c>
       <c r="K32" s="0"/>
       <c r="L32" s="0"/>
-      <c r="M32" s="35" t="s">
+      <c r="M32" s="0"/>
+      <c r="N32" s="35" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="36" t="n">
         <v>4</v>
       </c>
@@ -2312,16 +2352,19 @@
       <c r="I33" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="J33" s="37" t="s">
+      <c r="J33" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="K33" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="K33" s="37" t="s">
+      <c r="L33" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="L33" s="39" t="s">
+      <c r="M33" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="M33" s="35"/>
+      <c r="N33" s="35"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="36" t="n">
@@ -2331,7 +2374,7 @@
       <c r="C34" s="34"/>
       <c r="D34" s="34"/>
       <c r="E34" s="34"/>
-      <c r="M34" s="35"/>
+      <c r="N34" s="35"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="36" t="n">
@@ -2358,18 +2401,21 @@
       <c r="I35" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="J35" s="37" t="s">
+      <c r="J35" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K35" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="K35" s="37" t="s">
+      <c r="L35" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="L35" s="39" t="s">
+      <c r="M35" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="M35" s="35"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N35" s="35"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="36" t="n">
         <v>7</v>
       </c>
@@ -2394,12 +2440,15 @@
       <c r="I36" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="J36" s="0"/>
+      <c r="J36" s="27" t="s">
+        <v>85</v>
+      </c>
       <c r="K36" s="0"/>
       <c r="L36" s="0"/>
       <c r="M36" s="0"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="36" t="n">
         <v>8</v>
       </c>
@@ -2424,20 +2473,23 @@
       <c r="I37" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="J37" s="37" t="s">
+      <c r="J37" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="K37" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="K37" s="37" t="s">
+      <c r="L37" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="L37" s="39" t="s">
+      <c r="M37" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="M37" s="35" t="s">
+      <c r="N37" s="35" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="36" t="n">
         <v>9</v>
       </c>
@@ -2457,15 +2509,18 @@
         <v>84</v>
       </c>
       <c r="G38" s="34" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="I38" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="J38" s="0"/>
+      <c r="J38" s="40" t="s">
+        <v>106</v>
+      </c>
       <c r="K38" s="0"/>
       <c r="L38" s="0"/>
-      <c r="M38" s="35" t="s">
+      <c r="M38" s="0"/>
+      <c r="N38" s="35" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2477,7 +2532,7 @@
       <c r="C39" s="34"/>
       <c r="D39" s="34"/>
       <c r="E39" s="34"/>
-      <c r="M39" s="35"/>
+      <c r="N39" s="35"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="36" t="n">
@@ -2504,17 +2559,20 @@
       <c r="I40" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="J40" s="37" t="s">
+      <c r="J40" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K40" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="K40" s="37" t="s">
+      <c r="L40" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="L40" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="M40" s="35" t="s">
+      <c r="M40" s="15" t="s">
         <v>110</v>
+      </c>
+      <c r="N40" s="35" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2542,17 +2600,20 @@
       <c r="I41" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="J41" s="37" t="s">
+      <c r="J41" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K41" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="K41" s="37" t="s">
+      <c r="L41" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="L41" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="M41" s="35" t="s">
-        <v>111</v>
+      <c r="M41" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="N41" s="35" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2580,17 +2641,20 @@
       <c r="I42" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="J42" s="37" t="s">
+      <c r="J42" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K42" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="K42" s="37" t="s">
+      <c r="L42" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="L42" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="M42" s="35" t="s">
-        <v>111</v>
+      <c r="M42" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="N42" s="35" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2601,7 +2665,7 @@
       <c r="C43" s="34"/>
       <c r="D43" s="34"/>
       <c r="E43" s="34"/>
-      <c r="M43" s="35"/>
+      <c r="N43" s="35"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
@@ -2625,8 +2689,11 @@
       <c r="I44" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="M44" s="35" t="s">
-        <v>112</v>
+      <c r="J44" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="N44" s="35" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2651,8 +2718,11 @@
       <c r="I45" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="M45" s="35" t="s">
-        <v>113</v>
+      <c r="J45" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="N45" s="35" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2677,8 +2747,11 @@
       <c r="I46" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="M46" s="35" t="s">
-        <v>113</v>
+      <c r="J46" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="N46" s="35" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2689,9 +2762,9 @@
       <c r="C47" s="34"/>
       <c r="D47" s="34"/>
       <c r="E47" s="34"/>
-      <c r="M47" s="35"/>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N47" s="35"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
         <v>19</v>
       </c>
@@ -2705,7 +2778,7 @@
         <v>108</v>
       </c>
       <c r="E48" s="43" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F48" s="27" t="s">
         <v>85</v>
@@ -2713,9 +2786,12 @@
       <c r="I48" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="M48" s="35"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J48" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="N48" s="35"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
         <v>20</v>
       </c>
@@ -2729,7 +2805,7 @@
         <v>104</v>
       </c>
       <c r="E49" s="43" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F49" s="27" t="s">
         <v>83</v>
@@ -2737,9 +2813,12 @@
       <c r="I49" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="M49" s="35"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J49" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="N49" s="35"/>
+    </row>
+    <row r="50" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
         <v>21</v>
       </c>
@@ -2747,13 +2826,13 @@
         <v>103</v>
       </c>
       <c r="C50" s="37" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D50" s="37" t="s">
         <v>100</v>
       </c>
       <c r="E50" s="43" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F50" s="27" t="s">
         <v>83</v>
@@ -2761,9 +2840,12 @@
       <c r="I50" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="M50" s="35"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J50" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="N50" s="35"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
         <v>22</v>
       </c>
@@ -2777,7 +2859,7 @@
         <v>100</v>
       </c>
       <c r="E51" s="43" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F51" s="27" t="s">
         <v>85</v>
@@ -2785,9 +2867,12 @@
       <c r="I51" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="M51" s="35"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J51" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="N51" s="35"/>
+    </row>
+    <row r="52" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
         <v>23</v>
       </c>
@@ -2795,13 +2880,13 @@
         <v>7</v>
       </c>
       <c r="C52" s="37" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D52" s="37" t="s">
         <v>100</v>
       </c>
       <c r="E52" s="43" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F52" s="27" t="s">
         <v>83</v>
@@ -2809,7 +2894,10 @@
       <c r="I52" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="M52" s="35"/>
+      <c r="J52" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="N52" s="35"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
@@ -2819,9 +2907,9 @@
       <c r="C53" s="34"/>
       <c r="D53" s="34"/>
       <c r="E53" s="34"/>
-      <c r="M53" s="35"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N53" s="35"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
         <v>25</v>
       </c>
@@ -2841,19 +2929,22 @@
         <v>85</v>
       </c>
       <c r="G54" s="27" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I54" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="M54" s="27" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J54" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="N54" s="27" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
         <v>26</v>
       </c>
@@ -2873,15 +2964,18 @@
         <v>85</v>
       </c>
       <c r="G55" s="27" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H55" s="27" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I55" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="M55" s="35"/>
+      <c r="J55" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="N55" s="35"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
@@ -2894,7 +2988,7 @@
       <c r="F56" s="0"/>
       <c r="G56" s="0"/>
       <c r="H56" s="0"/>
-      <c r="M56" s="35"/>
+      <c r="N56" s="35"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
@@ -2904,7 +2998,7 @@
       <c r="C57" s="37"/>
       <c r="D57" s="37"/>
       <c r="E57" s="34"/>
-      <c r="M57" s="35"/>
+      <c r="N57" s="35"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
@@ -2914,10 +3008,10 @@
       <c r="C58" s="37"/>
       <c r="D58" s="37"/>
       <c r="E58" s="34"/>
-      <c r="K58" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="M58" s="35"/>
+      <c r="L58" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="N58" s="35"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
@@ -2927,7 +3021,7 @@
       <c r="C59" s="37"/>
       <c r="D59" s="37"/>
       <c r="E59" s="34"/>
-      <c r="M59" s="35"/>
+      <c r="N59" s="35"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
@@ -2937,7 +3031,7 @@
       <c r="C60" s="37"/>
       <c r="D60" s="37"/>
       <c r="E60" s="34"/>
-      <c r="M60" s="35"/>
+      <c r="N60" s="35"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
@@ -2947,7 +3041,7 @@
       <c r="C61" s="37"/>
       <c r="D61" s="37"/>
       <c r="E61" s="34"/>
-      <c r="M61" s="35"/>
+      <c r="N61" s="35"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
@@ -2957,7 +3051,7 @@
       <c r="C62" s="37"/>
       <c r="D62" s="37"/>
       <c r="E62" s="34"/>
-      <c r="M62" s="35"/>
+      <c r="N62" s="35"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
@@ -2967,20 +3061,20 @@
       <c r="C63" s="37"/>
       <c r="D63" s="37"/>
       <c r="E63" s="34"/>
-      <c r="M63" s="35"/>
-    </row>
-    <row r="64" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N63" s="35"/>
+    </row>
+    <row r="64" s="10" customFormat="true" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
         <v>35</v>
       </c>
       <c r="B64" s="41" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C64" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D64" s="41" t="s">
         <v>122</v>
-      </c>
-      <c r="D64" s="41" t="s">
-        <v>121</v>
       </c>
       <c r="E64" s="44" t="s">
         <v>43</v>
@@ -2993,26 +3087,29 @@
         <v>85</v>
       </c>
       <c r="I64" s="35"/>
-      <c r="J64" s="35"/>
+      <c r="J64" s="40" t="s">
+        <v>106</v>
+      </c>
       <c r="K64" s="35"/>
       <c r="L64" s="35"/>
-      <c r="M64" s="35" t="s">
-        <v>123</v>
-      </c>
-      <c r="N64" s="35"/>
+      <c r="M64" s="35"/>
+      <c r="N64" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="O64" s="35"/>
     </row>
     <row r="65" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
         <v>36</v>
       </c>
       <c r="B65" s="41" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C65" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D65" s="41" t="s">
         <v>122</v>
-      </c>
-      <c r="D65" s="41" t="s">
-        <v>121</v>
       </c>
       <c r="E65" s="44" t="s">
         <v>44</v>
@@ -3025,26 +3122,29 @@
         <v>85</v>
       </c>
       <c r="I65" s="35"/>
-      <c r="J65" s="35"/>
+      <c r="J65" s="27" t="s">
+        <v>85</v>
+      </c>
       <c r="K65" s="35"/>
       <c r="L65" s="35"/>
-      <c r="M65" s="35" t="s">
-        <v>124</v>
-      </c>
-      <c r="N65" s="35"/>
+      <c r="M65" s="35"/>
+      <c r="N65" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="O65" s="35"/>
     </row>
     <row r="66" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
         <v>37</v>
       </c>
       <c r="B66" s="41" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C66" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D66" s="41" t="s">
         <v>122</v>
-      </c>
-      <c r="D66" s="41" t="s">
-        <v>121</v>
       </c>
       <c r="E66" s="44" t="s">
         <v>45</v>
@@ -3057,26 +3157,29 @@
         <v>85</v>
       </c>
       <c r="I66" s="35"/>
-      <c r="J66" s="35"/>
+      <c r="J66" s="27" t="s">
+        <v>85</v>
+      </c>
       <c r="K66" s="35"/>
       <c r="L66" s="35"/>
-      <c r="M66" s="35" t="s">
-        <v>124</v>
-      </c>
-      <c r="N66" s="35"/>
+      <c r="M66" s="35"/>
+      <c r="N66" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="O66" s="35"/>
     </row>
     <row r="67" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
         <v>38</v>
       </c>
       <c r="B67" s="41" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C67" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D67" s="41" t="s">
         <v>122</v>
-      </c>
-      <c r="D67" s="41" t="s">
-        <v>121</v>
       </c>
       <c r="E67" s="35" t="s">
         <v>46</v>
@@ -3086,29 +3189,32 @@
       </c>
       <c r="G67" s="35"/>
       <c r="H67" s="35" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I67" s="35"/>
-      <c r="J67" s="35"/>
+      <c r="J67" s="35" t="s">
+        <v>106</v>
+      </c>
       <c r="K67" s="35"/>
       <c r="L67" s="35"/>
-      <c r="M67" s="35" t="s">
-        <v>123</v>
-      </c>
-      <c r="N67" s="35"/>
+      <c r="M67" s="35"/>
+      <c r="N67" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="O67" s="35"/>
     </row>
     <row r="68" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
         <v>39</v>
       </c>
       <c r="B68" s="41" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C68" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D68" s="41" t="s">
         <v>122</v>
-      </c>
-      <c r="D68" s="41" t="s">
-        <v>121</v>
       </c>
       <c r="E68" s="35" t="s">
         <v>47</v>
@@ -3123,11 +3229,14 @@
       <c r="I68" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="J68" s="35"/>
+      <c r="J68" s="35" t="s">
+        <v>85</v>
+      </c>
       <c r="K68" s="35"/>
       <c r="L68" s="35"/>
       <c r="M68" s="35"/>
       <c r="N68" s="35"/>
+      <c r="O68" s="35"/>
     </row>
     <row r="69" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
@@ -3137,7 +3246,7 @@
         <v>103</v>
       </c>
       <c r="C69" s="41" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D69" s="41" t="s">
         <v>15</v>
@@ -3155,19 +3264,22 @@
       <c r="I69" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="J69" s="41" t="s">
-        <v>102</v>
+      <c r="J69" s="35" t="s">
+        <v>85</v>
       </c>
       <c r="K69" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="L69" s="46" t="s">
+      <c r="L69" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="M69" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="M69" s="35" t="s">
-        <v>123</v>
-      </c>
-      <c r="N69" s="35"/>
+      <c r="N69" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="O69" s="35"/>
     </row>
     <row r="70" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
@@ -3177,10 +3289,10 @@
         <v>103</v>
       </c>
       <c r="C70" s="41" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D70" s="41" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E70" s="45" t="s">
         <v>41</v>
@@ -3193,11 +3305,14 @@
         <v>85</v>
       </c>
       <c r="I70" s="35"/>
-      <c r="J70" s="35"/>
+      <c r="J70" s="27" t="s">
+        <v>85</v>
+      </c>
       <c r="K70" s="35"/>
       <c r="L70" s="35"/>
       <c r="M70" s="35"/>
       <c r="N70" s="35"/>
+      <c r="O70" s="35"/>
     </row>
     <row r="71" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
@@ -3207,10 +3322,10 @@
         <v>7</v>
       </c>
       <c r="C71" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D71" s="41" t="s">
         <v>122</v>
-      </c>
-      <c r="D71" s="41" t="s">
-        <v>121</v>
       </c>
       <c r="E71" s="45" t="s">
         <v>41</v>
@@ -3223,24 +3338,27 @@
         <v>83</v>
       </c>
       <c r="I71" s="35"/>
-      <c r="J71" s="35"/>
+      <c r="J71" s="27" t="s">
+        <v>85</v>
+      </c>
       <c r="K71" s="35"/>
       <c r="L71" s="35"/>
       <c r="M71" s="35"/>
       <c r="N71" s="35"/>
-    </row>
-    <row r="72" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O71" s="35"/>
+    </row>
+    <row r="72" s="10" customFormat="true" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
         <v>43</v>
       </c>
       <c r="B72" s="41" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C72" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D72" s="41" t="s">
         <v>122</v>
-      </c>
-      <c r="D72" s="41" t="s">
-        <v>121</v>
       </c>
       <c r="E72" s="47" t="s">
         <v>42</v>
@@ -3253,13 +3371,16 @@
         <v>83</v>
       </c>
       <c r="I72" s="35"/>
-      <c r="J72" s="35"/>
+      <c r="J72" s="40" t="s">
+        <v>106</v>
+      </c>
       <c r="K72" s="35"/>
       <c r="L72" s="35"/>
-      <c r="M72" s="35" t="s">
-        <v>123</v>
-      </c>
-      <c r="N72" s="35"/>
+      <c r="M72" s="35"/>
+      <c r="N72" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="O72" s="35"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
@@ -3275,13 +3396,13 @@
         <v>45</v>
       </c>
       <c r="B74" s="37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C74" s="37" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D74" s="37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E74" s="34" t="s">
         <v>43</v>
@@ -3289,19 +3410,22 @@
       <c r="F74" s="27" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J74" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
         <v>46</v>
       </c>
       <c r="B75" s="37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C75" s="37" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D75" s="37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E75" s="34" t="s">
         <v>44</v>
@@ -3309,19 +3433,22 @@
       <c r="F75" s="27" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J75" s="40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
         <v>47</v>
       </c>
       <c r="B76" s="37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C76" s="37" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D76" s="37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E76" s="34" t="s">
         <v>45</v>
@@ -3329,19 +3456,22 @@
       <c r="F76" s="27" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J76" s="40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
         <v>48</v>
       </c>
       <c r="B77" s="37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C77" s="37" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D77" s="37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E77" s="27" t="s">
         <v>46</v>
@@ -3349,19 +3479,22 @@
       <c r="F77" s="27" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J77" s="40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
         <v>49</v>
       </c>
       <c r="B78" s="37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C78" s="37" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D78" s="37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E78" s="27" t="s">
         <v>47</v>
@@ -3369,19 +3502,22 @@
       <c r="F78" s="27" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J78" s="40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
         <v>50</v>
       </c>
       <c r="B79" s="37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C79" s="37" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D79" s="37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E79" s="15" t="s">
         <v>41</v>
@@ -3389,25 +3525,31 @@
       <c r="F79" s="27" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J79" s="40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
         <v>51</v>
       </c>
       <c r="B80" s="37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C80" s="37" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D80" s="37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E80" s="11" t="s">
         <v>42</v>
       </c>
       <c r="F80" s="27" t="s">
         <v>83</v>
+      </c>
+      <c r="J80" s="40" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3419,15 +3561,15 @@
       <c r="D81" s="37"/>
       <c r="E81" s="11"/>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
         <v>53</v>
       </c>
       <c r="C82" s="41" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D82" s="41" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E82" s="44" t="s">
         <v>43</v>
@@ -3441,23 +3583,26 @@
       <c r="I82" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="J82" s="37" t="s">
+      <c r="J82" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K82" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="K82" s="37"/>
-      <c r="L82" s="37" t="s">
+      <c r="L82" s="37"/>
+      <c r="M82" s="37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
         <v>54</v>
       </c>
       <c r="C83" s="41" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D83" s="41" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E83" s="44" t="s">
         <v>44</v>
@@ -3472,21 +3617,24 @@
         <v>106</v>
       </c>
       <c r="J83" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K83" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="L83" s="37" t="s">
+      <c r="M83" s="37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
         <v>55</v>
       </c>
       <c r="C84" s="41" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D84" s="41" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E84" s="44" t="s">
         <v>45</v>
@@ -3500,16 +3648,19 @@
       <c r="I84" s="40" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J84" s="27" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
         <v>56</v>
       </c>
       <c r="C85" s="41" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D85" s="41" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E85" s="35" t="s">
         <v>46</v>
@@ -3523,19 +3674,22 @@
       <c r="I85" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="M85" s="27" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J85" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="N85" s="27" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
         <v>57</v>
       </c>
       <c r="C86" s="41" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D86" s="41" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E86" s="35" t="s">
         <v>47</v>
@@ -3549,16 +3703,19 @@
       <c r="I86" s="40" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J86" s="27" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
         <v>58</v>
       </c>
       <c r="C87" s="41" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D87" s="41" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E87" s="45" t="s">
         <v>41</v>
@@ -3572,26 +3729,29 @@
       <c r="I87" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="J87" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="K87" s="37"/>
-      <c r="L87" s="27" t="s">
-        <v>130</v>
-      </c>
+      <c r="J87" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K87" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="L87" s="37"/>
       <c r="M87" s="27" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N87" s="27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
         <v>59</v>
       </c>
       <c r="C88" s="41" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D88" s="41" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E88" s="47" t="s">
         <v>42</v>
@@ -3604,6 +3764,9 @@
       </c>
       <c r="I88" s="40" t="s">
         <v>106</v>
+      </c>
+      <c r="J88" s="27" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3622,6 +3785,7 @@
       <c r="L89" s="0"/>
       <c r="M89" s="0"/>
       <c r="N89" s="0"/>
+      <c r="O89" s="0"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="36" t="n">
@@ -3631,10 +3795,10 @@
         <v>7</v>
       </c>
       <c r="C90" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D90" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E90" s="34" t="s">
         <v>43</v>
@@ -3648,8 +3812,11 @@
       <c r="I90" s="27" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J90" s="27" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="36" t="n">
         <v>62</v>
       </c>
@@ -3657,10 +3824,10 @@
         <v>7</v>
       </c>
       <c r="C91" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D91" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E91" s="34" t="s">
         <v>44</v>
@@ -3675,13 +3842,16 @@
         <v>106</v>
       </c>
       <c r="J91" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K91" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="L91" s="37" t="s">
+      <c r="M91" s="37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="36" t="n">
         <v>63</v>
       </c>
@@ -3689,10 +3859,10 @@
         <v>7</v>
       </c>
       <c r="C92" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D92" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E92" s="34" t="s">
         <v>45</v>
@@ -3707,9 +3877,12 @@
         <v>106</v>
       </c>
       <c r="J92" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="L92" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="K92" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="M92" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3721,10 +3894,10 @@
         <v>7</v>
       </c>
       <c r="C93" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D93" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E93" s="27" t="s">
         <v>46</v>
@@ -3738,7 +3911,10 @@
       <c r="I93" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="L93" s="37"/>
+      <c r="J93" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="M93" s="37"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="36" t="n">
@@ -3748,10 +3924,10 @@
         <v>7</v>
       </c>
       <c r="C94" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D94" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E94" s="27" t="s">
         <v>47</v>
@@ -3765,13 +3941,16 @@
       <c r="I94" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="J94" s="0"/>
+      <c r="J94" s="27" t="s">
+        <v>85</v>
+      </c>
       <c r="K94" s="0"/>
-      <c r="L94" s="37" t="s">
+      <c r="L94" s="0"/>
+      <c r="M94" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="M94" s="27" t="s">
-        <v>134</v>
+      <c r="N94" s="27" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3782,10 +3961,10 @@
         <v>7</v>
       </c>
       <c r="C95" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D95" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E95" s="15" t="s">
         <v>41</v>
@@ -3797,6 +3976,9 @@
         <v>83</v>
       </c>
       <c r="I95" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J95" s="27" t="s">
         <v>85</v>
       </c>
     </row>
@@ -3808,10 +3990,10 @@
         <v>7</v>
       </c>
       <c r="C96" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D96" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E96" s="11" t="s">
         <v>42</v>
@@ -3823,6 +4005,9 @@
         <v>83</v>
       </c>
       <c r="I96" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J96" s="27" t="s">
         <v>85</v>
       </c>
     </row>
@@ -3834,13 +4019,13 @@
         <v>7</v>
       </c>
       <c r="C97" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D97" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E97" s="27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F97" s="27" t="s">
         <v>83</v>
@@ -3851,8 +4036,11 @@
       <c r="I97" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="M97" s="27" t="s">
-        <v>136</v>
+      <c r="J97" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="N97" s="27" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3863,13 +4051,13 @@
         <v>7</v>
       </c>
       <c r="C98" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D98" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E98" s="38" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F98" s="27" t="s">
         <v>83</v>
@@ -3878,6 +4066,9 @@
         <v>83</v>
       </c>
       <c r="I98" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J98" s="27" t="s">
         <v>85</v>
       </c>
     </row>
@@ -3889,10 +4080,10 @@
         <v>7</v>
       </c>
       <c r="C99" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D99" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E99" s="27" t="s">
         <v>48</v>
@@ -3907,13 +4098,16 @@
         <v>85</v>
       </c>
       <c r="J99" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K99" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="L99" s="37" t="s">
+      <c r="M99" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="M99" s="27" t="s">
-        <v>138</v>
+      <c r="N99" s="27" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3924,10 +4118,10 @@
         <v>7</v>
       </c>
       <c r="C100" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D100" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E100" s="27" t="s">
         <v>49</v>
@@ -3941,8 +4135,11 @@
       <c r="I100" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="M100" s="27" t="s">
-        <v>136</v>
+      <c r="J100" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="N100" s="27" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3961,6 +4158,7 @@
       <c r="L101" s="0"/>
       <c r="M101" s="0"/>
       <c r="N101" s="0"/>
+      <c r="O101" s="0"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="36" t="n">
@@ -3970,7 +4168,7 @@
         <v>103</v>
       </c>
       <c r="C102" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D102" s="0" t="s">
         <v>8</v>
@@ -3988,9 +4186,12 @@
         <v>85</v>
       </c>
       <c r="J102" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="L102" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="K102" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="M102" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4002,7 +4203,7 @@
         <v>103</v>
       </c>
       <c r="C103" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D103" s="0" t="s">
         <v>8</v>
@@ -4020,9 +4221,12 @@
         <v>85</v>
       </c>
       <c r="J103" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K103" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="L103" s="37" t="s">
+      <c r="M103" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4034,7 +4238,7 @@
         <v>103</v>
       </c>
       <c r="C104" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D104" s="0" t="s">
         <v>8</v>
@@ -4052,9 +4256,12 @@
         <v>85</v>
       </c>
       <c r="J104" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="L104" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="K104" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="M104" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4066,7 +4273,7 @@
         <v>103</v>
       </c>
       <c r="C105" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D105" s="0" t="s">
         <v>8</v>
@@ -4081,6 +4288,9 @@
         <v>83</v>
       </c>
       <c r="I105" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J105" s="27" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4092,7 +4302,7 @@
         <v>103</v>
       </c>
       <c r="C106" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D106" s="0" t="s">
         <v>8</v>
@@ -4109,15 +4319,18 @@
       <c r="I106" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="J106" s="37" t="s">
-        <v>140</v>
-      </c>
-      <c r="K106" s="37"/>
-      <c r="L106" s="37" t="s">
+      <c r="J106" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K106" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="M106" s="27" t="s">
+      <c r="L106" s="37"/>
+      <c r="M106" s="37" t="s">
         <v>142</v>
+      </c>
+      <c r="N106" s="27" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4128,7 +4341,7 @@
         <v>103</v>
       </c>
       <c r="C107" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D107" s="0" t="s">
         <v>8</v>
@@ -4145,8 +4358,11 @@
       <c r="I107" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="M107" s="27" t="s">
-        <v>143</v>
+      <c r="J107" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="N107" s="27" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4157,7 +4373,7 @@
         <v>103</v>
       </c>
       <c r="C108" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D108" s="0" t="s">
         <v>8</v>
@@ -4172,6 +4388,9 @@
         <v>83</v>
       </c>
       <c r="I108" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J108" s="27" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4183,13 +4402,13 @@
         <v>103</v>
       </c>
       <c r="C109" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D109" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E109" s="27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F109" s="27" t="s">
         <v>83</v>
@@ -4200,8 +4419,11 @@
       <c r="I109" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="M109" s="27" t="s">
-        <v>136</v>
+      <c r="J109" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="N109" s="27" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4212,13 +4434,13 @@
         <v>103</v>
       </c>
       <c r="C110" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D110" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E110" s="38" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F110" s="27" t="s">
         <v>85</v>
@@ -4230,13 +4452,16 @@
         <v>85</v>
       </c>
       <c r="J110" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="L110" s="27" t="s">
-        <v>144</v>
+        <v>85</v>
+      </c>
+      <c r="K110" s="27" t="s">
+        <v>140</v>
       </c>
       <c r="M110" s="27" t="s">
         <v>145</v>
+      </c>
+      <c r="N110" s="27" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4247,7 +4472,7 @@
         <v>103</v>
       </c>
       <c r="C111" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D111" s="0" t="s">
         <v>8</v>
@@ -4265,13 +4490,16 @@
         <v>85</v>
       </c>
       <c r="J111" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K111" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="L111" s="37" t="s">
+      <c r="M111" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="M111" s="27" t="s">
-        <v>146</v>
+      <c r="N111" s="27" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4282,7 +4510,7 @@
         <v>103</v>
       </c>
       <c r="C112" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D112" s="0" t="s">
         <v>8</v>
@@ -4299,8 +4527,11 @@
       <c r="I112" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="M112" s="27" t="s">
-        <v>136</v>
+      <c r="J112" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="N112" s="27" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4319,6 +4550,7 @@
       <c r="L113" s="0"/>
       <c r="M113" s="0"/>
       <c r="N113" s="0"/>
+      <c r="O113" s="0"/>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="36" t="n">
@@ -4328,10 +4560,10 @@
         <v>7</v>
       </c>
       <c r="C114" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D114" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E114" s="34" t="s">
         <v>43</v>
@@ -4343,6 +4575,9 @@
         <v>83</v>
       </c>
       <c r="I114" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J114" s="27" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4354,10 +4589,10 @@
         <v>7</v>
       </c>
       <c r="C115" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D115" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E115" s="34" t="s">
         <v>44</v>
@@ -4369,6 +4604,9 @@
         <v>83</v>
       </c>
       <c r="I115" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J115" s="27" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4380,10 +4618,10 @@
         <v>7</v>
       </c>
       <c r="C116" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D116" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E116" s="34" t="s">
         <v>45</v>
@@ -4395,6 +4633,9 @@
         <v>83</v>
       </c>
       <c r="I116" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J116" s="27" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4406,10 +4647,10 @@
         <v>7</v>
       </c>
       <c r="C117" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D117" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E117" s="27" t="s">
         <v>46</v>
@@ -4421,6 +4662,9 @@
         <v>83</v>
       </c>
       <c r="I117" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J117" s="27" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4432,10 +4676,10 @@
         <v>7</v>
       </c>
       <c r="C118" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D118" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E118" s="27" t="s">
         <v>47</v>
@@ -4449,8 +4693,11 @@
       <c r="I118" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="M118" s="27" t="s">
-        <v>148</v>
+      <c r="J118" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="N118" s="27" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4461,10 +4708,10 @@
         <v>7</v>
       </c>
       <c r="C119" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D119" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E119" s="15" t="s">
         <v>41</v>
@@ -4476,6 +4723,9 @@
         <v>83</v>
       </c>
       <c r="I119" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J119" s="27" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4487,10 +4737,10 @@
         <v>7</v>
       </c>
       <c r="C120" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D120" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E120" s="11" t="s">
         <v>42</v>
@@ -4502,6 +4752,9 @@
         <v>83</v>
       </c>
       <c r="I120" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J120" s="27" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4513,31 +4766,34 @@
         <v>7</v>
       </c>
       <c r="C121" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D121" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E121" s="27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F121" s="27" t="s">
         <v>83</v>
       </c>
       <c r="H121" s="27" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I121" s="27" t="s">
         <v>85</v>
       </c>
       <c r="J121" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K121" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="L121" s="27" t="s">
+      <c r="M121" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="M121" s="27" t="s">
-        <v>150</v>
+      <c r="N121" s="27" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4548,13 +4804,13 @@
         <v>7</v>
       </c>
       <c r="C122" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D122" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E122" s="38" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F122" s="27" t="s">
         <v>83</v>
@@ -4563,6 +4819,9 @@
         <v>83</v>
       </c>
       <c r="I122" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J122" s="27" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4574,31 +4833,34 @@
         <v>7</v>
       </c>
       <c r="C123" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D123" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E123" s="27" t="s">
         <v>48</v>
       </c>
       <c r="F123" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="H123" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="I123" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J123" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K123" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="M123" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="N123" s="27" t="s">
         <v>151</v>
-      </c>
-      <c r="H123" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="I123" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="J123" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="L123" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="M123" s="27" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4609,31 +4871,34 @@
         <v>7</v>
       </c>
       <c r="C124" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D124" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E124" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="F124" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="F124" s="27" t="s">
+      <c r="H124" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="I124" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J124" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K124" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="M124" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="N124" s="27" t="s">
         <v>151</v>
-      </c>
-      <c r="H124" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="I124" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="J124" s="27" t="s">
-        <v>153</v>
-      </c>
-      <c r="L124" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="M124" s="27" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4651,7 +4916,7 @@
         <v>103</v>
       </c>
       <c r="C126" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D126" s="0" t="s">
         <v>8</v>
@@ -4663,13 +4928,16 @@
         <v>85</v>
       </c>
       <c r="H126" s="27" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I126" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="M126" s="27" t="s">
-        <v>155</v>
+      <c r="J126" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="N126" s="27" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4680,7 +4948,7 @@
         <v>103</v>
       </c>
       <c r="C127" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D127" s="0" t="s">
         <v>8</v>
@@ -4695,6 +4963,9 @@
         <v>83</v>
       </c>
       <c r="I127" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J127" s="27" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4706,7 +4977,7 @@
         <v>103</v>
       </c>
       <c r="C128" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D128" s="0" t="s">
         <v>8</v>
@@ -4721,6 +4992,9 @@
         <v>83</v>
       </c>
       <c r="I128" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J128" s="27" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4732,7 +5006,7 @@
         <v>103</v>
       </c>
       <c r="C129" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D129" s="0" t="s">
         <v>8</v>
@@ -4747,6 +5021,9 @@
         <v>83</v>
       </c>
       <c r="I129" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J129" s="27" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4758,7 +5035,7 @@
         <v>103</v>
       </c>
       <c r="C130" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D130" s="0" t="s">
         <v>8</v>
@@ -4775,8 +5052,11 @@
       <c r="I130" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="M130" s="27" t="s">
-        <v>148</v>
+      <c r="J130" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="N130" s="27" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4787,7 +5067,7 @@
         <v>103</v>
       </c>
       <c r="C131" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D131" s="0" t="s">
         <v>8</v>
@@ -4802,6 +5082,9 @@
         <v>83</v>
       </c>
       <c r="I131" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J131" s="27" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4813,7 +5096,7 @@
         <v>103</v>
       </c>
       <c r="C132" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D132" s="0" t="s">
         <v>8</v>
@@ -4828,6 +5111,9 @@
         <v>83</v>
       </c>
       <c r="I132" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J132" s="27" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4839,31 +5125,34 @@
         <v>103</v>
       </c>
       <c r="C133" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D133" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E133" s="27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F133" s="27" t="s">
         <v>83</v>
       </c>
       <c r="H133" s="27" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I133" s="27" t="s">
         <v>85</v>
       </c>
       <c r="J133" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K133" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="L133" s="27" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M133" s="27" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="36" t="n">
         <v>105</v>
       </c>
@@ -4871,13 +5160,13 @@
         <v>103</v>
       </c>
       <c r="C134" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D134" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E134" s="38" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F134" s="27" t="s">
         <v>85</v>
@@ -4889,13 +5178,16 @@
         <v>106</v>
       </c>
       <c r="J134" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K134" s="27" t="s">
         <v>23</v>
-      </c>
-      <c r="L134" s="27" t="s">
-        <v>144</v>
       </c>
       <c r="M134" s="27" t="s">
         <v>145</v>
+      </c>
+      <c r="N134" s="27" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4906,7 +5198,7 @@
         <v>103</v>
       </c>
       <c r="C135" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D135" s="0" t="s">
         <v>8</v>
@@ -4915,22 +5207,25 @@
         <v>48</v>
       </c>
       <c r="F135" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="H135" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="I135" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J135" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K135" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="M135" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="N135" s="27" t="s">
         <v>151</v>
-      </c>
-      <c r="H135" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="I135" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="J135" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="L135" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="M135" s="27" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4941,31 +5236,34 @@
         <v>103</v>
       </c>
       <c r="C136" s="48" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D136" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E136" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="F136" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="F136" s="27" t="s">
+      <c r="H136" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="I136" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J136" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K136" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="M136" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="N136" s="27" t="s">
         <v>151</v>
-      </c>
-      <c r="H136" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="I136" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="J136" s="27" t="s">
-        <v>153</v>
-      </c>
-      <c r="L136" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="M136" s="27" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4983,7 +5281,7 @@
         <v>103</v>
       </c>
       <c r="C138" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D138" s="37" t="s">
         <v>104</v>
@@ -5000,11 +5298,14 @@
       <c r="I138" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="J138" s="37" t="s">
+      <c r="J138" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K138" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="K138" s="37"/>
-      <c r="L138" s="37" t="s">
+      <c r="L138" s="37"/>
+      <c r="M138" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -5016,7 +5317,7 @@
         <v>103</v>
       </c>
       <c r="C139" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D139" s="37" t="s">
         <v>104</v>
@@ -5034,9 +5335,12 @@
         <v>85</v>
       </c>
       <c r="J139" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K139" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="L139" s="37" t="s">
+      <c r="M139" s="37" t="s">
         <v>7</v>
       </c>
     </row>
@@ -5048,7 +5352,7 @@
         <v>103</v>
       </c>
       <c r="C140" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D140" s="37" t="s">
         <v>104</v>
@@ -5066,13 +5370,16 @@
         <v>85</v>
       </c>
       <c r="J140" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="L140" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="K140" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="M140" s="37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="36" t="n">
         <v>112</v>
       </c>
@@ -5080,7 +5387,7 @@
         <v>13</v>
       </c>
       <c r="C141" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D141" s="37" t="s">
         <v>104</v>
@@ -5097,17 +5404,20 @@
       <c r="I141" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="J141" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="L141" s="27" t="s">
+      <c r="J141" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="K141" s="27" t="s">
         <v>157</v>
       </c>
       <c r="M141" s="27" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N141" s="27" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="36" t="n">
         <v>113</v>
       </c>
@@ -5115,7 +5425,7 @@
         <v>19</v>
       </c>
       <c r="C142" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D142" s="37" t="s">
         <v>104</v>
@@ -5129,8 +5439,11 @@
       <c r="I142" s="40" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J142" s="40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="36" t="n">
         <v>114</v>
       </c>
@@ -5138,7 +5451,7 @@
         <v>103</v>
       </c>
       <c r="C143" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D143" s="37" t="s">
         <v>104</v>
@@ -5156,10 +5469,13 @@
         <v>106</v>
       </c>
       <c r="J143" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="M143" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K143" s="27" t="s">
         <v>160</v>
+      </c>
+      <c r="N143" s="27" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5170,7 +5486,7 @@
         <v>103</v>
       </c>
       <c r="C144" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D144" s="37" t="s">
         <v>104</v>
@@ -5187,12 +5503,15 @@
       <c r="I144" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="J144" s="37" t="s">
+      <c r="J144" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K144" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="K144" s="37"/>
-      <c r="L144" s="27" t="s">
-        <v>130</v>
+      <c r="L144" s="37"/>
+      <c r="M144" s="27" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5203,7 +5522,7 @@
         <v>103</v>
       </c>
       <c r="C145" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D145" s="37" t="s">
         <v>104</v>
@@ -5218,6 +5537,9 @@
         <v>83</v>
       </c>
       <c r="I145" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J145" s="27" t="s">
         <v>85</v>
       </c>
     </row>
@@ -5229,7 +5551,7 @@
         <v>103</v>
       </c>
       <c r="C146" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D146" s="37" t="s">
         <v>104</v>
@@ -5238,22 +5560,25 @@
         <v>48</v>
       </c>
       <c r="F146" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="H146" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="I146" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J146" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K146" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="M146" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="N146" s="27" t="s">
         <v>151</v>
-      </c>
-      <c r="H146" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="I146" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="J146" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="L146" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="M146" s="27" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5264,13 +5589,13 @@
         <v>103</v>
       </c>
       <c r="C147" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D147" s="37" t="s">
         <v>104</v>
       </c>
       <c r="E147" s="27" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F147" s="27" t="s">
         <v>83</v>
@@ -5279,6 +5604,9 @@
         <v>83</v>
       </c>
       <c r="I147" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J147" s="27" t="s">
         <v>85</v>
       </c>
     </row>
@@ -5297,7 +5625,7 @@
         <v>103</v>
       </c>
       <c r="C149" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D149" s="48" t="s">
         <v>21</v>
@@ -5315,13 +5643,16 @@
         <v>85</v>
       </c>
       <c r="J149" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K149" s="27" t="s">
         <v>22</v>
-      </c>
-      <c r="L149" s="27" t="s">
-        <v>161</v>
       </c>
       <c r="M149" s="27" t="s">
         <v>162</v>
+      </c>
+      <c r="N149" s="27" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5332,7 +5663,7 @@
         <v>103</v>
       </c>
       <c r="C150" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D150" s="48" t="s">
         <v>21</v>
@@ -5350,13 +5681,16 @@
         <v>85</v>
       </c>
       <c r="J150" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K150" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="L150" s="27" t="s">
-        <v>161</v>
-      </c>
       <c r="M150" s="27" t="s">
-        <v>163</v>
+        <v>162</v>
+      </c>
+      <c r="N150" s="27" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5367,7 +5701,7 @@
         <v>103</v>
       </c>
       <c r="C151" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D151" s="48" t="s">
         <v>21</v>
@@ -5385,16 +5719,19 @@
         <v>85</v>
       </c>
       <c r="J151" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="L151" s="27" t="s">
-        <v>161</v>
+        <v>85</v>
+      </c>
+      <c r="K151" s="27" t="s">
+        <v>134</v>
       </c>
       <c r="M151" s="27" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>162</v>
+      </c>
+      <c r="N151" s="27" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="36" t="n">
         <v>123</v>
       </c>
@@ -5402,7 +5739,7 @@
         <v>13</v>
       </c>
       <c r="C152" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D152" s="48" t="s">
         <v>21</v>
@@ -5419,17 +5756,20 @@
       <c r="I152" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="J152" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="L152" s="27" t="s">
+      <c r="J152" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="K152" s="27" t="s">
         <v>157</v>
       </c>
       <c r="M152" s="27" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>158</v>
+      </c>
+      <c r="N152" s="27" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="36" t="n">
         <v>124</v>
       </c>
@@ -5437,7 +5777,7 @@
         <v>19</v>
       </c>
       <c r="C153" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D153" s="48" t="s">
         <v>21</v>
@@ -5451,8 +5791,11 @@
       <c r="I153" s="40" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J153" s="40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="36" t="n">
         <v>125</v>
       </c>
@@ -5460,7 +5803,7 @@
         <v>103</v>
       </c>
       <c r="C154" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D154" s="48" t="s">
         <v>21</v>
@@ -5477,8 +5820,11 @@
       <c r="I154" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="M154" s="27" t="s">
-        <v>166</v>
+      <c r="J154" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="N154" s="27" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5489,7 +5835,7 @@
         <v>103</v>
       </c>
       <c r="C155" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D155" s="48" t="s">
         <v>21</v>
@@ -5504,6 +5850,9 @@
         <v>83</v>
       </c>
       <c r="I155" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J155" s="27" t="s">
         <v>85</v>
       </c>
     </row>
@@ -5515,7 +5864,7 @@
         <v>103</v>
       </c>
       <c r="C156" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D156" s="48" t="s">
         <v>21</v>
@@ -5533,10 +5882,13 @@
         <v>85</v>
       </c>
       <c r="J156" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="L156" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K156" s="27" t="s">
         <v>157</v>
+      </c>
+      <c r="M156" s="27" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5547,7 +5899,7 @@
         <v>103</v>
       </c>
       <c r="C157" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D157" s="48" t="s">
         <v>21</v>
@@ -5556,22 +5908,25 @@
         <v>48</v>
       </c>
       <c r="F157" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="H157" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="I157" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J157" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K157" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="M157" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="N157" s="27" t="s">
         <v>151</v>
-      </c>
-      <c r="H157" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="I157" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="J157" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="L157" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="M157" s="27" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5582,13 +5937,13 @@
         <v>103</v>
       </c>
       <c r="C158" s="37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D158" s="48" t="s">
         <v>21</v>
       </c>
       <c r="E158" s="27" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F158" s="27" t="s">
         <v>83</v>
@@ -5597,6 +5952,9 @@
         <v>83</v>
       </c>
       <c r="I158" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J158" s="27" t="s">
         <v>85</v>
       </c>
     </row>
@@ -5666,7 +6024,7 @@
       <c r="E172" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="B29:N172"/>
+  <autoFilter ref="B29:O172"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -5689,7 +6047,7 @@
       <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.18"/>
@@ -5699,170 +6057,170 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="C31" s="0" t="s">
         <v>205</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -5887,7 +6245,7 @@
       <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.07"/>
@@ -5895,158 +6253,158 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="27" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="27"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="27" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="27" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D3" s="27"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="27" t="s">
         <v>216</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>215</v>
       </c>
       <c r="D4" s="27"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="27" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D5" s="27"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C6" s="27" t="s">
         <v>219</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>218</v>
       </c>
       <c r="D6" s="27"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="27" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D7" s="27"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="27" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="27" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="27" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C10" s="27"/>
       <c r="D10" s="27" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="27" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C11" s="27"/>
       <c r="D11" s="27" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>